<commit_message>
Added Done Point enumeration and Test Sequence Template
</commit_message>
<xml_diff>
--- a/Project Template/2 Architecture/Major Component BOM Template.xlsx
+++ b/Project Template/2 Architecture/Major Component BOM Template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="2360" yWindow="1640" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Major Components " sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>Project</t>
   </si>
@@ -131,8 +131,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -142,9 +144,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -635,10 +639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -812,8 +816,56 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>